<commit_message>
ajustados parametros de impressão
</commit_message>
<xml_diff>
--- a/src/escala_ASO1.xlsx
+++ b/src/escala_ASO1.xlsx
@@ -8,7 +8,9 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Escala" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName localSheetId="0" name="_xlnm.Print_Area">Escala!$A$1:$AG$15</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -413,7 +415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AG15"/>
   <sheetViews>
@@ -1349,6 +1351,6 @@
     <mergeCell ref="A1:AG1"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>